<commit_message>
Production Planning Draft Done
</commit_message>
<xml_diff>
--- a/3.4 Production Planning/Group 02_WS_25-26 M3 Prodution Planning.xlsx
+++ b/3.4 Production Planning/Group 02_WS_25-26 M3 Prodution Planning.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\HSRW\Semester 5\Group Project\Group-Project_WS2526\3.4 Production Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A602C641-6EF4-454C-9BDF-37AA24F097EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A41799C-BEFA-453A-AC77-7B079157D52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{DE72B6C7-421C-4069-887E-620521B1C591}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" firstSheet="6" activeTab="6" xr2:uid="{DE72B6C7-421C-4069-887E-620521B1C591}"/>
   </bookViews>
   <sheets>
     <sheet name="takt-time" sheetId="2" r:id="rId1"/>
     <sheet name="machine-efficiency" sheetId="3" r:id="rId2"/>
     <sheet name="production-time" sheetId="4" r:id="rId3"/>
     <sheet name="machine-allocation" sheetId="6" r:id="rId4"/>
-    <sheet name="production-time-calc" sheetId="5" r:id="rId5"/>
+    <sheet name="workforce" sheetId="8" r:id="rId5"/>
+    <sheet name="production-time-calc" sheetId="5" r:id="rId6"/>
+    <sheet name="assembly-stations" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="192">
   <si>
     <t>Year 1</t>
   </si>
@@ -204,15 +206,9 @@
     <t>Backward Extrusion and 4-axis CNC Milling</t>
   </si>
   <si>
-    <t>Fiber Glass Laser cutting and Welding</t>
-  </si>
-  <si>
     <t>3-axis CNC Milling</t>
   </si>
   <si>
-    <t>Drilling and Reaming</t>
-  </si>
-  <si>
     <t>Soldering</t>
   </si>
   <si>
@@ -276,17 +272,469 @@
     <t>Machine Availability [min/year]</t>
   </si>
   <si>
-    <t>Required prodution Time</t>
-  </si>
-  <si>
     <t>No. of Machines (estimate)</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Processing Time Per Unit [min/unit]</t>
+  </si>
+  <si>
+    <t>Setup Time Per Unit [min/unit]</t>
+  </si>
+  <si>
+    <t>Transfering between stations</t>
+  </si>
+  <si>
+    <t>0.2mm layer, quality, 30% infill w/ supportts</t>
+  </si>
+  <si>
+    <t>0.2mm layer, quality, 70% infill w/ supportts</t>
+  </si>
+  <si>
+    <t>Secure workpiece</t>
+  </si>
+  <si>
+    <t>Loading laser cutter</t>
+  </si>
+  <si>
+    <t>Laser cutting</t>
+  </si>
+  <si>
+    <t>Collect workpieces</t>
+  </si>
+  <si>
+    <t>Setup and secure workpieces</t>
+  </si>
+  <si>
+    <t>Weld work pieces</t>
+  </si>
+  <si>
+    <t>Extrusion Process</t>
+  </si>
+  <si>
+    <t>Remove workpiece</t>
+  </si>
+  <si>
+    <t>Rotating (x4)</t>
+  </si>
+  <si>
+    <t>Milling groves (x4)</t>
+  </si>
+  <si>
+    <t>Milling hole</t>
+  </si>
+  <si>
+    <t>Finishing (x4) w/ grinder</t>
+  </si>
+  <si>
+    <t>Transfer piece to CNC Mill</t>
+  </si>
+  <si>
+    <t>Reaming</t>
+  </si>
+  <si>
+    <t>Required prodution Time per year [min/year]</t>
+  </si>
+  <si>
+    <t>Total Time [min/unit]</t>
+  </si>
+  <si>
+    <t>PRODUCTION</t>
+  </si>
+  <si>
+    <t>ASSEMBLY</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>Top Panel and Tray</t>
+  </si>
+  <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>Basin + Panel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secure PCB in stencil </t>
+  </si>
+  <si>
+    <t>Apply solder paste</t>
+  </si>
+  <si>
+    <t>Remove from stencil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secure PCB into pnp </t>
+  </si>
+  <si>
+    <t>PnP places all components</t>
+  </si>
+  <si>
+    <t>Remove from pnp</t>
+  </si>
+  <si>
+    <t>Secure in Oven</t>
+  </si>
+  <si>
+    <t>Reflow in Oven</t>
+  </si>
+  <si>
+    <t>Remove from Oven (+cooling)</t>
+  </si>
+  <si>
+    <t>Weld</t>
+  </si>
+  <si>
+    <t>Hand solder THT components</t>
+  </si>
+  <si>
+    <t>MACHINES</t>
+  </si>
+  <si>
+    <t>Required Workers</t>
+  </si>
+  <si>
+    <t>Required Production Time [min/day]</t>
+  </si>
+  <si>
+    <t>Required Shifts [shifts/day]</t>
+  </si>
+  <si>
+    <t>Required prodution Time per unit [min/unit]</t>
+  </si>
+  <si>
+    <t>Assembly Station</t>
+  </si>
+  <si>
+    <t>Sub assembly station</t>
+  </si>
+  <si>
+    <t>Parts assembly</t>
+  </si>
+  <si>
+    <t>Assembly Process</t>
+  </si>
+  <si>
+    <t>Total Time (mins)</t>
+  </si>
+  <si>
+    <t>Expected Worker</t>
+  </si>
+  <si>
+    <t>Line 1 – Basin Assembly</t>
+  </si>
+  <si>
+    <t>Line 1.1 – PCB Assembly (A1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part 1 and all electrical components (Table 27, except USB C and M12 port) </t>
+  </si>
+  <si>
+    <t>Place solder paste using stencil</t>
+  </si>
+  <si>
+    <t>Place all components (Automated pick and place machine)</t>
+  </si>
+  <si>
+    <t>Solder (Reflow oven)</t>
+  </si>
+  <si>
+    <t>Line 1.2 – PCB mount assembly (A3)</t>
+  </si>
+  <si>
+    <t>1, 2, 16 and 22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Screw PCB into Mount </t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Line 1.3 – Battery Cradle Assembly (A2)</t>
+  </si>
+  <si>
+    <t>3 and 25</t>
+  </si>
+  <si>
+    <t>Strap Velcro onto cradle</t>
+  </si>
+  <si>
+    <t>Line 1.4 –</t>
+  </si>
+  <si>
+    <t>Battery cradle into basin (A6)</t>
+  </si>
+  <si>
+    <t>2, 7, 17 and 21</t>
+  </si>
+  <si>
+    <t>Screw the battery cradle in</t>
+  </si>
+  <si>
+    <t>Line 1.5 – M12 port into basin (A8)</t>
+  </si>
+  <si>
+    <r>
+      <t>7, 13 and M12 gasket</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Insert M12 port into the basin</t>
+  </si>
+  <si>
+    <t>Line 1.6 – PCB Mount into basin (A7)</t>
+  </si>
+  <si>
+    <r>
+      <t>2, 7 and 27</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Tape the PCB mount onto the wall</t>
+  </si>
+  <si>
+    <t>Line 1.7 – Frame and gasket onto basin (A9 &amp; A10)</t>
+  </si>
+  <si>
+    <r>
+      <t>7, 8, Battery, 17</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, 21, 24 and 26</t>
+    </r>
+  </si>
+  <si>
+    <t>Place in the battery, then place gasket and screw frame on to the basin</t>
+  </si>
+  <si>
+    <t>Line 2 – Top Panel Assembly</t>
+  </si>
+  <si>
+    <t>Line 2.1 – Top Panel welding (A4)</t>
+  </si>
+  <si>
+    <t>9 and 10</t>
+  </si>
+  <si>
+    <t>Weld cable tray onto top panel</t>
+  </si>
+  <si>
+    <t>Line 2.2 – Buttons and ports insertion</t>
+  </si>
+  <si>
+    <t>SW1, SW2, J2, D2, 9, 18 and 24</t>
+  </si>
+  <si>
+    <t>Screw the buttons, LEDs and USB A port into the top panel</t>
+  </si>
+  <si>
+    <t>Line 3 – Electronics interior assembly</t>
+  </si>
+  <si>
+    <t>Line 3.1 – Top panel and basin assembly (A11)</t>
+  </si>
+  <si>
+    <t>7 and 9</t>
+  </si>
+  <si>
+    <t>Weld top panel and basin together</t>
+  </si>
+  <si>
+    <t>Line 3.2 – Screen insertion (A12)</t>
+  </si>
+  <si>
+    <r>
+      <t>7, EDPM Foam tape</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and U12</t>
+    </r>
+  </si>
+  <si>
+    <t>Insert screen and tape for sealing</t>
+  </si>
+  <si>
+    <t>Line 4 – Panel frame assembly</t>
+  </si>
+  <si>
+    <t>(A14)</t>
+  </si>
+  <si>
+    <r>
+      <t>4 and 20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>  </t>
+    </r>
+  </si>
+  <si>
+    <t>Insert rivets into panel frame</t>
+  </si>
+  <si>
+    <t>Line 5 – Pelican case assembly</t>
+  </si>
+  <si>
+    <t>Line 5.1 – USB C port insertion (A13)</t>
+  </si>
+  <si>
+    <r>
+      <t>J3 and 12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Insert USB – C port </t>
+  </si>
+  <si>
+    <t>Line 5.2 – screw in panel frame (A15 &amp; A16)</t>
+  </si>
+  <si>
+    <r>
+      <t>4, 5, 6, 11, 12 and 19 and glue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Insert foam into case, then screw in panel frame</t>
+  </si>
+  <si>
+    <t>Line 5.3 – electronics insertion (A17)</t>
+  </si>
+  <si>
+    <r>
+      <t>7, 12 and O-ring</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Screw in electronics with O-ring</t>
+  </si>
+  <si>
+    <t>Line 6 – Final assembly</t>
+  </si>
+  <si>
+    <t>A18</t>
+  </si>
+  <si>
+    <t>12 and load cells and cables</t>
+  </si>
+  <si>
+    <t>Keep the load cells and cables in and close the box</t>
+  </si>
+  <si>
+    <t>Assembly Time [min/unit]</t>
+  </si>
+  <si>
+    <t>WORKFORCE</t>
+  </si>
+  <si>
+    <t>Assembly Lines</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>Y2</t>
+  </si>
+  <si>
+    <t>Y3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="172" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,6 +787,25 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -354,7 +821,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -515,11 +982,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -595,7 +1095,7 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -643,6 +1143,94 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="4" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="4" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -980,8 +1568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F2B21B-7A31-4FF1-A341-071C71BDA9A3}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1141,7 +1729,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A13"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1242,7 +1830,7 @@
         <v>79380</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>21</v>
       </c>
@@ -1299,7 +1887,7 @@
         <v>56700</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="22" t="s">
         <v>24</v>
       </c>
@@ -1318,7 +1906,7 @@
         <v>79380</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
         <v>25</v>
       </c>
@@ -1337,7 +1925,7 @@
         <v>56700</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="94.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="22" t="s">
         <v>26</v>
       </c>
@@ -1356,7 +1944,7 @@
         <v>85050</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
         <v>27</v>
       </c>
@@ -1375,7 +1963,7 @@
         <v>96390</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="22" t="s">
         <v>28</v>
       </c>
@@ -1401,10 +1989,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A63EC935-1910-457F-AF5E-DDCB700C53A2}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1417,7 +2005,7 @@
     <col min="11" max="11" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>29</v>
       </c>
@@ -1428,10 +2016,10 @@
         <v>44</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F1" s="38" t="s">
         <v>46</v>
@@ -1443,7 +2031,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="25">
         <v>1</v>
       </c>
@@ -1454,28 +2042,27 @@
         <v>49</v>
       </c>
       <c r="D2" s="42">
+        <f>'production-time-calc'!E4</f>
         <v>102</v>
       </c>
       <c r="E2" s="42">
-        <v>20</v>
+        <f>'production-time-calc'!F4</f>
+        <v>15</v>
       </c>
       <c r="F2" s="39">
         <f>D2+E2</f>
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G2" s="39">
         <v>150</v>
       </c>
       <c r="H2" s="39">
         <f>F2*G2</f>
-        <v>18300</v>
+        <v>17550</v>
       </c>
       <c r="I2" s="17"/>
-      <c r="L2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="14">
         <v>2</v>
       </c>
@@ -1486,32 +2073,27 @@
         <v>50</v>
       </c>
       <c r="D3" s="43">
-        <v>60</v>
+        <f>'production-time-calc'!E11</f>
+        <v>193</v>
       </c>
       <c r="E3" s="43">
-        <v>15</v>
+        <f>'production-time-calc'!F11</f>
+        <v>2</v>
       </c>
       <c r="F3" s="39">
         <f t="shared" ref="F3:F14" si="0">D3+E3</f>
-        <v>75</v>
+        <v>195</v>
       </c>
       <c r="G3" s="39">
         <v>150</v>
       </c>
       <c r="H3" s="39">
         <f t="shared" ref="H3:H14" si="1">F3*G3</f>
-        <v>11250</v>
+        <v>29250</v>
       </c>
       <c r="I3" s="22"/>
-      <c r="K3" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="44">
-        <f>SUM(H3,H4)</f>
-        <v>19500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="25">
         <v>3</v>
       </c>
@@ -1522,32 +2104,27 @@
         <v>50</v>
       </c>
       <c r="D4" s="42">
-        <v>45</v>
+        <f>'production-time-calc'!E13</f>
+        <v>202</v>
       </c>
       <c r="E4" s="42">
-        <v>10</v>
+        <f>'production-time-calc'!F13</f>
+        <v>5</v>
       </c>
       <c r="F4" s="39">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>207</v>
       </c>
       <c r="G4" s="39">
         <v>150</v>
       </c>
       <c r="H4" s="39">
         <f t="shared" si="1"/>
-        <v>8250</v>
+        <v>31050</v>
       </c>
       <c r="I4" s="17"/>
-      <c r="K4" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4">
-        <f>H5+H8/2</f>
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="26">
         <v>4</v>
       </c>
@@ -1558,32 +2135,27 @@
         <v>51</v>
       </c>
       <c r="D5" s="43">
+        <f>'production-time-calc'!E15</f>
         <v>30</v>
       </c>
       <c r="E5" s="43">
-        <v>20</v>
+        <f>'production-time-calc'!F15</f>
+        <v>16</v>
       </c>
       <c r="F5" s="39">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G5" s="39">
         <v>150</v>
       </c>
       <c r="H5" s="39">
         <f t="shared" si="1"/>
-        <v>7500</v>
+        <v>6900</v>
       </c>
       <c r="I5" s="22"/>
-      <c r="K5" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="44">
-        <f>H6+H7+H12</f>
-        <v>10200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:9" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="25">
         <v>5</v>
       </c>
@@ -1594,32 +2166,27 @@
         <v>52</v>
       </c>
       <c r="D6" s="42">
-        <v>25</v>
+        <f>'production-time-calc'!E23</f>
+        <v>35</v>
       </c>
       <c r="E6" s="42">
-        <v>15</v>
+        <f>'production-time-calc'!F23</f>
+        <v>10</v>
       </c>
       <c r="F6" s="39">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G6" s="39">
         <v>150</v>
       </c>
       <c r="H6" s="39">
         <f t="shared" si="1"/>
-        <v>6000</v>
+        <v>6750</v>
       </c>
       <c r="I6" s="17"/>
-      <c r="K6" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" s="44">
-        <f>H10+H11</f>
-        <v>8250</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:9" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="26">
         <v>6</v>
       </c>
@@ -1630,32 +2197,27 @@
         <v>52</v>
       </c>
       <c r="D7" s="43">
-        <v>10</v>
+        <f>'production-time-calc'!E24</f>
+        <v>60</v>
       </c>
       <c r="E7" s="43">
-        <v>5</v>
+        <f>'production-time-calc'!F24</f>
+        <v>15</v>
       </c>
       <c r="F7" s="39">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="G7" s="39">
         <v>150</v>
       </c>
       <c r="H7" s="39">
         <f t="shared" si="1"/>
-        <v>2250</v>
+        <v>11250</v>
       </c>
       <c r="I7" s="22"/>
-      <c r="K7" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="L7">
-        <f>H8/2</f>
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:9" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="25">
         <v>7</v>
       </c>
@@ -1666,32 +2228,27 @@
         <v>53</v>
       </c>
       <c r="D8" s="42">
-        <v>30</v>
+        <f>'production-time-calc'!E25</f>
+        <v>74</v>
       </c>
       <c r="E8" s="42">
-        <v>30</v>
+        <f>'production-time-calc'!F25</f>
+        <v>60</v>
       </c>
       <c r="F8" s="39">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>134</v>
       </c>
       <c r="G8" s="39">
         <v>150</v>
       </c>
       <c r="H8" s="39">
         <f t="shared" si="1"/>
-        <v>9000</v>
+        <v>20100</v>
       </c>
       <c r="I8" s="17"/>
-      <c r="K8" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="L8">
-        <f>H13*70</f>
-        <v>231000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:9" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="26">
         <v>8</v>
       </c>
@@ -1699,35 +2256,30 @@
         <v>37</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D9" s="43">
-        <v>35</v>
+        <f>'production-time-calc'!E33</f>
+        <v>40</v>
       </c>
       <c r="E9" s="43">
-        <v>25</v>
+        <f>'production-time-calc'!F33</f>
+        <v>30</v>
       </c>
       <c r="F9" s="39">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="G9" s="39">
         <v>150</v>
       </c>
       <c r="H9" s="39">
         <f t="shared" si="1"/>
-        <v>9000</v>
+        <v>10500</v>
       </c>
       <c r="I9" s="22"/>
-      <c r="K9" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9">
-        <f>H13*0.3</f>
-        <v>990</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -1735,35 +2287,30 @@
         <v>38</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" s="42">
-        <v>20</v>
+        <f>'production-time-calc'!E38</f>
+        <v>40</v>
       </c>
       <c r="E10" s="42">
-        <v>10</v>
+        <f>'production-time-calc'!F38</f>
+        <v>25</v>
       </c>
       <c r="F10" s="39">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="G10" s="39">
         <v>150</v>
       </c>
       <c r="H10" s="39">
         <f t="shared" si="1"/>
-        <v>4500</v>
+        <v>9750</v>
       </c>
       <c r="I10" s="17"/>
-      <c r="K10" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="L10">
-        <f>H9*30</f>
-        <v>270000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="26">
         <v>10</v>
       </c>
@@ -1771,35 +2318,30 @@
         <v>39</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" s="43">
-        <v>15</v>
+        <f>'production-time-calc'!E39</f>
+        <v>20</v>
       </c>
       <c r="E11" s="43">
+        <f>'production-time-calc'!F39</f>
         <v>10</v>
       </c>
       <c r="F11" s="39">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G11" s="39">
         <v>150</v>
       </c>
       <c r="H11" s="39">
         <f t="shared" si="1"/>
-        <v>3750</v>
+        <v>4500</v>
       </c>
       <c r="I11" s="22"/>
-      <c r="K11" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="L11">
-        <f>H9*70</f>
-        <v>630000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -1810,9 +2352,11 @@
         <v>52</v>
       </c>
       <c r="D12" s="42">
+        <f>'production-time-calc'!E40</f>
         <v>8</v>
       </c>
       <c r="E12" s="42">
+        <f>'production-time-calc'!F40</f>
         <v>5</v>
       </c>
       <c r="F12" s="39">
@@ -1827,11 +2371,8 @@
         <v>1950</v>
       </c>
       <c r="I12" s="17"/>
-      <c r="K12" s="22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:9" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="26">
         <v>12</v>
       </c>
@@ -1839,31 +2380,30 @@
         <v>41</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D13" s="43">
-        <v>12</v>
+        <f>'production-time-calc'!E41</f>
+        <v>10</v>
       </c>
       <c r="E13" s="43">
+        <f>'production-time-calc'!F41</f>
         <v>10</v>
       </c>
       <c r="F13" s="39">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G13" s="39">
         <v>150</v>
       </c>
       <c r="H13" s="39">
         <f t="shared" si="1"/>
-        <v>3300</v>
+        <v>3000</v>
       </c>
       <c r="I13" s="22"/>
-      <c r="K13" s="17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:9" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="25">
         <v>13</v>
       </c>
@@ -1871,12 +2411,14 @@
         <v>43</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D14" s="42">
+        <f>'production-time-calc'!E44</f>
         <v>10</v>
       </c>
       <c r="E14" s="42">
+        <f>'production-time-calc'!F44</f>
         <v>5</v>
       </c>
       <c r="F14" s="39">
@@ -1891,12 +2433,11 @@
         <v>2250</v>
       </c>
       <c r="I14" s="27"/>
-      <c r="K14" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="L14" s="44">
-        <f>H14</f>
-        <v>2250</v>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F15" s="44">
+        <f>SUM(F2:F14)</f>
+        <v>1032</v>
       </c>
     </row>
   </sheetData>
@@ -1908,8 +2449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDED109F-8A36-4D93-A359-56271D892B16}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1925,16 +2466,16 @@
         <v>12</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>76</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1942,8 +2483,8 @@
         <v>17</v>
       </c>
       <c r="B2" s="45">
-        <f>'production-time'!L3</f>
-        <v>19500</v>
+        <f>'production-time-calc'!D49</f>
+        <v>60300</v>
       </c>
       <c r="C2" s="21">
         <f>'machine-efficiency'!E2</f>
@@ -1955,7 +2496,7 @@
       </c>
       <c r="E2" s="21">
         <f>B2/C2</f>
-        <v>0.31265031265031262</v>
+        <v>0.96681096681096668</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -1963,8 +2504,8 @@
         <v>18</v>
       </c>
       <c r="B3" s="45">
-        <f>'production-time'!L4</f>
-        <v>12000</v>
+        <f>'production-time-calc'!D50</f>
+        <v>24450</v>
       </c>
       <c r="C3" s="21">
         <f>'machine-efficiency'!E3</f>
@@ -1976,7 +2517,7 @@
       </c>
       <c r="E3" s="21">
         <f t="shared" ref="E3:E13" si="1">B3/C3</f>
-        <v>0.15117157974300832</v>
+        <v>0.30801209372637944</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -1984,8 +2525,8 @@
         <v>19</v>
       </c>
       <c r="B4" s="45">
-        <f>'production-time'!L5</f>
-        <v>10200</v>
+        <f>'production-time-calc'!D51</f>
+        <v>19950</v>
       </c>
       <c r="C4" s="21">
         <f>'machine-efficiency'!E4</f>
@@ -1997,7 +2538,7 @@
       </c>
       <c r="E4" s="21">
         <f t="shared" si="1"/>
-        <v>0.13838013838013838</v>
+        <v>0.27065527065527067</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -2005,8 +2546,8 @@
         <v>20</v>
       </c>
       <c r="B5" s="45">
-        <f>'production-time'!L6</f>
-        <v>8250</v>
+        <f>'production-time-calc'!D52</f>
+        <v>14250</v>
       </c>
       <c r="C5" s="21">
         <f>'machine-efficiency'!E5</f>
@@ -2018,7 +2559,7 @@
       </c>
       <c r="E5" s="21">
         <f t="shared" si="1"/>
-        <v>0.10393046107331821</v>
+        <v>0.17951625094482238</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2026,8 +2567,8 @@
         <v>21</v>
       </c>
       <c r="B6" s="45">
-        <f>'production-time'!L7</f>
-        <v>4500</v>
+        <f>'production-time-calc'!D53</f>
+        <v>2550</v>
       </c>
       <c r="C6" s="21">
         <f>'machine-efficiency'!E6</f>
@@ -2039,7 +2580,7 @@
       </c>
       <c r="E6" s="21">
         <f t="shared" si="1"/>
-        <v>4.4091710758377423E-2</v>
+        <v>2.4985302763080541E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2047,8 +2588,8 @@
         <v>22</v>
       </c>
       <c r="B7" s="45">
-        <f>'production-time'!L8</f>
-        <v>231000</v>
+        <f>'production-time-calc'!D54</f>
+        <v>2100</v>
       </c>
       <c r="C7" s="21">
         <f>'machine-efficiency'!E7</f>
@@ -2056,11 +2597,11 @@
       </c>
       <c r="D7" s="21">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E7" s="21">
         <f t="shared" si="1"/>
-        <v>3.3950617283950617</v>
+        <v>3.0864197530864196E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2068,8 +2609,8 @@
         <v>23</v>
       </c>
       <c r="B8" s="45">
-        <f>'production-time'!L9</f>
-        <v>990</v>
+        <f>'production-time-calc'!D55</f>
+        <v>2400</v>
       </c>
       <c r="C8" s="21">
         <f>'machine-efficiency'!E8</f>
@@ -2081,7 +2622,7 @@
       </c>
       <c r="E8" s="21">
         <f t="shared" si="1"/>
-        <v>1.7460317460317461E-2</v>
+        <v>4.2328042328042326E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2089,8 +2630,8 @@
         <v>24</v>
       </c>
       <c r="B9" s="45">
-        <f>'production-time'!L10</f>
-        <v>270000</v>
+        <f>'production-time-calc'!D56</f>
+        <v>3750</v>
       </c>
       <c r="C9" s="21">
         <f>'machine-efficiency'!E9</f>
@@ -2098,11 +2639,11 @@
       </c>
       <c r="D9" s="21">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E9" s="21">
         <f t="shared" si="1"/>
-        <v>3.4013605442176869</v>
+        <v>4.7241118669690101E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2110,8 +2651,8 @@
         <v>25</v>
       </c>
       <c r="B10" s="45">
-        <f>'production-time'!L11</f>
-        <v>630000</v>
+        <f>'production-time-calc'!D57</f>
+        <v>11550</v>
       </c>
       <c r="C10" s="21">
         <f>'machine-efficiency'!E10</f>
@@ -2119,11 +2660,11 @@
       </c>
       <c r="D10" s="21">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E10" s="21">
         <f t="shared" si="1"/>
-        <v>11.111111111111111</v>
+        <v>0.20370370370370369</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -2131,8 +2672,8 @@
         <v>26</v>
       </c>
       <c r="B11" s="45">
-        <f>'production-time'!L12</f>
-        <v>0</v>
+        <f>'production-time-calc'!D58</f>
+        <v>1650</v>
       </c>
       <c r="C11" s="21">
         <f>'machine-efficiency'!E11</f>
@@ -2140,11 +2681,11 @@
       </c>
       <c r="D11" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.9400352733686066E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2152,8 +2693,8 @@
         <v>27</v>
       </c>
       <c r="B12" s="45">
-        <f>'production-time'!L13</f>
-        <v>0</v>
+        <f>'production-time-calc'!D59</f>
+        <v>3075</v>
       </c>
       <c r="C12" s="21">
         <f>'machine-efficiency'!E12</f>
@@ -2161,11 +2702,11 @@
       </c>
       <c r="D12" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.1901649548708375E-2</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -2173,8 +2714,8 @@
         <v>28</v>
       </c>
       <c r="B13" s="45">
-        <f>'production-time'!L14</f>
-        <v>2250</v>
+        <f>'production-time-calc'!D60</f>
+        <v>3750</v>
       </c>
       <c r="C13" s="21">
         <f>'machine-efficiency'!E13</f>
@@ -2186,7 +2727,7 @@
       </c>
       <c r="E13" s="21">
         <f t="shared" si="1"/>
-        <v>5.6689342403628121E-2</v>
+        <v>9.4482237339380201E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2195,374 +2736,2048 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C67BB7A-75CF-4381-AF9B-516380362064}">
+  <dimension ref="A1:G30"/>
+  <sheetViews>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="4" max="6" width="22.44140625" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A1" s="48" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:7" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3" s="16"/>
+    </row>
+    <row r="4" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="21">
+        <f>'machine-allocation'!D2</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="74">
+        <f>'production-time-calc'!D49/252</f>
+        <v>239.28571428571428</v>
+      </c>
+      <c r="D4" s="73">
+        <f>C4/(7.5*60)</f>
+        <v>0.53174603174603174</v>
+      </c>
+      <c r="E4" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" spans="1:7" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="21">
+        <f>'machine-allocation'!D3</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="74">
+        <f>'production-time-calc'!D50/252</f>
+        <v>97.023809523809518</v>
+      </c>
+      <c r="D5" s="73">
+        <f t="shared" ref="D5:D13" si="0">C5/(7.5*60)</f>
+        <v>0.21560846560846558</v>
+      </c>
+      <c r="E5" s="21">
+        <f t="shared" ref="E5:E13" si="1">_xlfn.CEILING.MATH(D5)</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="21"/>
+      <c r="G5" s="24"/>
+    </row>
+    <row r="6" spans="1:7" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="21">
+        <f>'machine-allocation'!D4</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="74">
+        <f>'production-time-calc'!D51/252</f>
+        <v>79.166666666666671</v>
+      </c>
+      <c r="D6" s="73">
+        <f t="shared" si="0"/>
+        <v>0.17592592592592593</v>
+      </c>
+      <c r="E6" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+    </row>
+    <row r="7" spans="1:7" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="21">
+        <f>'machine-allocation'!D5</f>
+        <v>1</v>
+      </c>
+      <c r="C7" s="74">
+        <f>'production-time-calc'!D52/252</f>
+        <v>56.547619047619051</v>
+      </c>
+      <c r="D7" s="73">
+        <f t="shared" si="0"/>
+        <v>0.12566137566137567</v>
+      </c>
+      <c r="E7" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="21"/>
+    </row>
+    <row r="8" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="21">
+        <f>'machine-allocation'!D6</f>
+        <v>1</v>
+      </c>
+      <c r="C8" s="74">
+        <f>'production-time-calc'!D53/252</f>
+        <v>10.119047619047619</v>
+      </c>
+      <c r="D8" s="73">
+        <f t="shared" si="0"/>
+        <v>2.2486772486772486E-2</v>
+      </c>
+      <c r="E8" s="21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F8" s="21"/>
+    </row>
+    <row r="9" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="21">
+        <f>'machine-allocation'!D7</f>
+        <v>1</v>
+      </c>
+      <c r="C9" s="74">
+        <f>'production-time-calc'!D54/252</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="D9" s="73">
+        <f t="shared" si="0"/>
+        <v>1.8518518518518521E-2</v>
+      </c>
+      <c r="E9" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="21"/>
+    </row>
+    <row r="10" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="21">
+        <f>'machine-allocation'!D8</f>
+        <v>1</v>
+      </c>
+      <c r="C10" s="74">
+        <f>'production-time-calc'!D55/252</f>
+        <v>9.5238095238095237</v>
+      </c>
+      <c r="D10" s="73">
+        <f t="shared" si="0"/>
+        <v>2.1164021164021163E-2</v>
+      </c>
+      <c r="E10" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="21"/>
+    </row>
+    <row r="11" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="21">
+        <f>'machine-allocation'!D9</f>
+        <v>1</v>
+      </c>
+      <c r="C11" s="74">
+        <f>'production-time-calc'!D56/252</f>
+        <v>14.880952380952381</v>
+      </c>
+      <c r="D11" s="73">
+        <f t="shared" si="0"/>
+        <v>3.3068783068783067E-2</v>
+      </c>
+      <c r="E11" s="21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F11" s="21"/>
+    </row>
+    <row r="12" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="21">
+        <f>'machine-allocation'!D10</f>
+        <v>1</v>
+      </c>
+      <c r="C12" s="74">
+        <f>'production-time-calc'!D57/252</f>
+        <v>45.833333333333336</v>
+      </c>
+      <c r="D12" s="73">
+        <f t="shared" si="0"/>
+        <v>0.10185185185185186</v>
+      </c>
+      <c r="E12" s="21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F12" s="21"/>
+    </row>
+    <row r="13" spans="1:7" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="21">
+        <f>'machine-allocation'!D13</f>
+        <v>1</v>
+      </c>
+      <c r="C13" s="74">
+        <f>'production-time-calc'!D58/252</f>
+        <v>6.5476190476190474</v>
+      </c>
+      <c r="D13" s="73">
+        <f t="shared" si="0"/>
+        <v>1.4550264550264549E-2</v>
+      </c>
+      <c r="E13" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="21"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <f>SUM(E4:E13)</f>
+        <v>7</v>
+      </c>
+      <c r="F14" s="72"/>
+    </row>
+    <row r="19" spans="1:4" ht="37.200000000000003" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A19" s="48" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="51" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="71" t="s">
+        <v>128</v>
+      </c>
+      <c r="B21" s="70">
+        <f>SUM('assembly-stations'!F4:F13)</f>
+        <v>58</v>
+      </c>
+      <c r="C21" s="70">
+        <v>0.5</v>
+      </c>
+      <c r="D21" s="21"/>
+    </row>
+    <row r="22" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="B22" s="54">
+        <f>SUM('assembly-stations'!F14:F15)</f>
+        <v>18</v>
+      </c>
+      <c r="C22" s="54">
+        <f>'assembly-stations'!G14</f>
+        <v>1</v>
+      </c>
+      <c r="D22" s="21"/>
+    </row>
+    <row r="23" spans="1:4" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="B23" s="54">
+        <f>'assembly-stations'!F16+'assembly-stations'!F17</f>
+        <v>19</v>
+      </c>
+      <c r="C23" s="54">
+        <f>'assembly-stations'!G16</f>
+        <v>1</v>
+      </c>
+      <c r="D23" s="21"/>
+    </row>
+    <row r="24" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="B24" s="54">
+        <f>'assembly-stations'!F18</f>
+        <v>3</v>
+      </c>
+      <c r="C24" s="54">
+        <f>'assembly-stations'!G18</f>
+        <v>1</v>
+      </c>
+      <c r="D24" s="21"/>
+    </row>
+    <row r="25" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B25" s="28">
+        <f>SUM('assembly-stations'!F19:F21)</f>
+        <v>7</v>
+      </c>
+      <c r="C25" s="28">
+        <f>'assembly-stations'!G19</f>
+        <v>2</v>
+      </c>
+      <c r="D25" s="21"/>
+    </row>
+    <row r="26" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="B26" s="54">
+        <f>'assembly-stations'!F22</f>
+        <v>2</v>
+      </c>
+      <c r="C26" s="54">
+        <f>'assembly-stations'!G22</f>
+        <v>1</v>
+      </c>
+      <c r="D26" s="21"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="69"/>
+      <c r="C27">
+        <f>SUM(C21:C26)</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A29" s="48" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f>C27+E14</f>
+        <v>13.5</v>
+      </c>
+      <c r="B30">
+        <v>13</v>
+      </c>
+      <c r="C30">
+        <f>B30*252*7.5</f>
+        <v>24570</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{899BBE11-0677-4B41-9774-F63CAC91108D}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:K79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.44140625" customWidth="1"/>
     <col min="3" max="4" width="27.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.21875" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" customWidth="1"/>
+    <col min="5" max="7" width="12.21875" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" customWidth="1"/>
+    <col min="16" max="16" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="63" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:11" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A1" s="48" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:11" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B3" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C3" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="K3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="25">
+        <v>1</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="25">
-        <v>1</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="41">
+      <c r="D4" s="41">
         <v>2</v>
       </c>
-      <c r="E2" s="41">
-        <f>SUM(D2:D7)</f>
+      <c r="E4" s="41">
+        <f>SUM(D4:D9)</f>
         <v>102</v>
       </c>
-      <c r="F2" s="17"/>
-    </row>
-    <row r="3" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="25"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="41">
-        <v>10</v>
-      </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="17"/>
-    </row>
-    <row r="4" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="25"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="41">
-        <v>40</v>
-      </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="17"/>
-    </row>
-    <row r="5" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F4" s="41">
+        <f>D10</f>
+        <v>15</v>
+      </c>
+      <c r="G4" s="41">
+        <f>E4+F4</f>
+        <v>117</v>
+      </c>
+      <c r="H4" s="17"/>
+    </row>
+    <row r="5" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25"/>
       <c r="B5" s="31"/>
       <c r="C5" s="32" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D5" s="41">
         <v>10</v>
       </c>
       <c r="E5" s="18"/>
-      <c r="F5" s="17"/>
-    </row>
-    <row r="6" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="17"/>
+    </row>
+    <row r="6" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="25"/>
       <c r="B6" s="31"/>
       <c r="C6" s="32" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="D6" s="41">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E6" s="18"/>
-      <c r="F6" s="17"/>
-    </row>
-    <row r="7" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="17"/>
+    </row>
+    <row r="7" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="25"/>
       <c r="B7" s="31"/>
       <c r="C7" s="32" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D7" s="41">
+        <v>10</v>
+      </c>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="17"/>
+    </row>
+    <row r="8" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="25"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="41">
         <v>20</v>
       </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="17"/>
-    </row>
-    <row r="8" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14">
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="17"/>
+    </row>
+    <row r="9" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="25"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="41">
+        <v>20</v>
+      </c>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="17"/>
+    </row>
+    <row r="10" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="25"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="41">
+        <v>15</v>
+      </c>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="17"/>
+    </row>
+    <row r="11" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="14">
         <v>2</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B11" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C11" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="22"/>
-    </row>
-    <row r="9" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="26"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="40"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="22"/>
-    </row>
-    <row r="10" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="25">
+      <c r="D11" s="40">
+        <v>193</v>
+      </c>
+      <c r="E11" s="41">
+        <f>SUM(D11)</f>
+        <v>193</v>
+      </c>
+      <c r="F11" s="41">
+        <f>D12</f>
+        <v>2</v>
+      </c>
+      <c r="G11" s="41">
+        <f>E11+F11</f>
+        <v>195</v>
+      </c>
+      <c r="H11" s="22"/>
+      <c r="K11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="26"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="40">
+        <v>2</v>
+      </c>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="22"/>
+    </row>
+    <row r="13" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="25">
         <v>3</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B13" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C13" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="17"/>
-    </row>
-    <row r="11" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="25"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="41"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="17"/>
-    </row>
-    <row r="12" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="26">
+      <c r="D13" s="41">
+        <v>202</v>
+      </c>
+      <c r="E13" s="41">
+        <f>SUM(D13)</f>
+        <v>202</v>
+      </c>
+      <c r="F13" s="41">
+        <f>D14</f>
+        <v>5</v>
+      </c>
+      <c r="G13" s="41">
+        <f>E13+F13</f>
+        <v>207</v>
+      </c>
+      <c r="H13" s="17"/>
+      <c r="K13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="25"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="41">
+        <v>5</v>
+      </c>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="17"/>
+    </row>
+    <row r="15" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="26">
         <v>4</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B15" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="22"/>
-    </row>
-    <row r="13" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="26"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="22"/>
-    </row>
-    <row r="14" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="26"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="22"/>
-    </row>
-    <row r="15" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="26"/>
-      <c r="B15" s="35"/>
       <c r="C15" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="22"/>
-    </row>
-    <row r="16" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+      <c r="D15" s="40">
+        <v>5</v>
+      </c>
+      <c r="E15" s="46">
+        <f>D16+D18+D20+D22</f>
+        <v>30</v>
+      </c>
+      <c r="F15" s="46">
+        <f>D15+D17+D19+D21</f>
+        <v>16</v>
+      </c>
+      <c r="G15" s="41">
+        <f>E15+F15</f>
+        <v>46</v>
+      </c>
+      <c r="H15" s="22"/>
+    </row>
+    <row r="16" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="26"/>
       <c r="B16" s="35"/>
       <c r="C16" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="40"/>
+        <v>64</v>
+      </c>
+      <c r="D16" s="40">
+        <v>6</v>
+      </c>
       <c r="E16" s="24"/>
-      <c r="F16" s="22"/>
-    </row>
-    <row r="17" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="22"/>
+    </row>
+    <row r="17" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="26"/>
       <c r="B17" s="35"/>
       <c r="C17" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="40"/>
+        <v>66</v>
+      </c>
+      <c r="D17" s="40">
+        <v>3</v>
+      </c>
       <c r="E17" s="24"/>
-      <c r="F17" s="22"/>
-    </row>
-    <row r="18" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="22"/>
+    </row>
+    <row r="18" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="26"/>
       <c r="B18" s="35"/>
       <c r="C18" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="40"/>
+        <v>65</v>
+      </c>
+      <c r="D18" s="40">
+        <v>18</v>
+      </c>
       <c r="E18" s="24"/>
-      <c r="F18" s="22"/>
-    </row>
-    <row r="19" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="25">
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="22"/>
+    </row>
+    <row r="19" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="26"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="40">
+        <v>4</v>
+      </c>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="22"/>
+    </row>
+    <row r="20" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="26"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="40">
+        <v>3</v>
+      </c>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="22"/>
+    </row>
+    <row r="21" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="26"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="40">
+        <v>4</v>
+      </c>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="22"/>
+    </row>
+    <row r="22" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="26"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="40">
+        <v>3</v>
+      </c>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="22"/>
+    </row>
+    <row r="23" spans="1:8" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="25">
         <v>5</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B23" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C23" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="41"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="17"/>
-    </row>
-    <row r="20" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="25"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="17"/>
-    </row>
-    <row r="21" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="26">
+      <c r="D23" s="41"/>
+      <c r="E23" s="28">
+        <v>35</v>
+      </c>
+      <c r="F23" s="28">
+        <v>10</v>
+      </c>
+      <c r="G23" s="41">
+        <f>E23+F23</f>
+        <v>45</v>
+      </c>
+      <c r="H23" s="17"/>
+    </row>
+    <row r="24" spans="1:8" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="26">
         <v>6</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B24" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="33" t="s">
+      <c r="C24" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="40"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="22"/>
-    </row>
-    <row r="22" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="25">
+      <c r="D24" s="40"/>
+      <c r="E24" s="24">
+        <v>60</v>
+      </c>
+      <c r="F24" s="24">
+        <v>15</v>
+      </c>
+      <c r="G24" s="41">
+        <f>E24+F24</f>
+        <v>75</v>
+      </c>
+      <c r="H24" s="22"/>
+    </row>
+    <row r="25" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="25">
         <v>7</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B25" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="41"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="17"/>
-    </row>
-    <row r="23" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="26">
-        <v>8</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="40"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="22"/>
-    </row>
-    <row r="24" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="25">
-        <v>9</v>
-      </c>
-      <c r="B24" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="41"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="17"/>
-    </row>
-    <row r="25" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="26">
+      <c r="C25" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="41">
         <v>10</v>
       </c>
-      <c r="B25" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="40"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="22"/>
-    </row>
-    <row r="26" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="25">
-        <v>11</v>
-      </c>
-      <c r="B26" s="31" t="s">
-        <v>40</v>
-      </c>
+      <c r="E25" s="47">
+        <f>D26+D29+D31+D32</f>
+        <v>74</v>
+      </c>
+      <c r="F25" s="47">
+        <f>D25+D27+D28+D30</f>
+        <v>60</v>
+      </c>
+      <c r="G25" s="41">
+        <f>E25+F25</f>
+        <v>134</v>
+      </c>
+      <c r="H25" s="17"/>
+    </row>
+    <row r="26" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="25"/>
+      <c r="B26" s="31"/>
       <c r="C26" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" s="41"/>
+        <v>89</v>
+      </c>
+      <c r="D26" s="41">
+        <v>2</v>
+      </c>
       <c r="E26" s="27"/>
-      <c r="F26" s="17"/>
-    </row>
-    <row r="27" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="26">
-        <v>12</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="40"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="22"/>
-    </row>
-    <row r="28" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="25">
-        <v>13</v>
-      </c>
-      <c r="B28" s="31" t="s">
-        <v>43</v>
-      </c>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="17"/>
+    </row>
+    <row r="27" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="25"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="41">
+        <v>5</v>
+      </c>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="17"/>
+    </row>
+    <row r="28" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="25"/>
+      <c r="B28" s="31"/>
       <c r="C28" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="41"/>
+        <v>95</v>
+      </c>
+      <c r="D28" s="41">
+        <v>25</v>
+      </c>
       <c r="E28" s="27"/>
       <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="17"/>
+    </row>
+    <row r="29" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="25"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="41">
+        <v>40</v>
+      </c>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="17"/>
+    </row>
+    <row r="30" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="25"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="41">
+        <v>20</v>
+      </c>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="17"/>
+    </row>
+    <row r="31" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="25"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" s="41">
+        <v>2</v>
+      </c>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="17"/>
+    </row>
+    <row r="32" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="25"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="41">
+        <v>30</v>
+      </c>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="17"/>
+    </row>
+    <row r="33" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="26">
+        <v>8</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" s="40">
+        <v>10</v>
+      </c>
+      <c r="E33" s="46">
+        <f>D34+D37</f>
+        <v>40</v>
+      </c>
+      <c r="F33" s="46">
+        <f>D33+D35+D36</f>
+        <v>30</v>
+      </c>
+      <c r="G33" s="41">
+        <f>E33+F33</f>
+        <v>70</v>
+      </c>
+      <c r="H33" s="22"/>
+    </row>
+    <row r="34" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="26"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="D34" s="40">
+        <v>10</v>
+      </c>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="22"/>
+    </row>
+    <row r="35" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="26"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="40">
+        <v>5</v>
+      </c>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="22"/>
+    </row>
+    <row r="36" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="26"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="40">
+        <v>15</v>
+      </c>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="22"/>
+    </row>
+    <row r="37" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="26"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D37" s="40">
+        <v>30</v>
+      </c>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="22"/>
+    </row>
+    <row r="38" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="25">
+        <v>9</v>
+      </c>
+      <c r="B38" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" s="41"/>
+      <c r="E38" s="27">
+        <v>40</v>
+      </c>
+      <c r="F38" s="27">
+        <v>25</v>
+      </c>
+      <c r="G38" s="41">
+        <f>E38+F38</f>
+        <v>65</v>
+      </c>
+      <c r="H38" s="17"/>
+    </row>
+    <row r="39" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="26">
+        <v>10</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="40"/>
+      <c r="E39" s="24">
+        <v>20</v>
+      </c>
+      <c r="F39" s="24">
+        <v>10</v>
+      </c>
+      <c r="G39" s="41">
+        <f>E39+F39</f>
+        <v>30</v>
+      </c>
+      <c r="H39" s="22"/>
+    </row>
+    <row r="40" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="25">
+        <v>11</v>
+      </c>
+      <c r="B40" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" s="41"/>
+      <c r="E40" s="27">
+        <v>8</v>
+      </c>
+      <c r="F40" s="27">
+        <v>5</v>
+      </c>
+      <c r="G40" s="41">
+        <f>E40+F40</f>
+        <v>13</v>
+      </c>
+      <c r="H40" s="17"/>
+    </row>
+    <row r="41" spans="1:8" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="26">
+        <v>12</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" s="40">
+        <v>10</v>
+      </c>
+      <c r="E41" s="46">
+        <f>D42+D43</f>
+        <v>10</v>
+      </c>
+      <c r="F41" s="46">
+        <f>D41</f>
+        <v>10</v>
+      </c>
+      <c r="G41" s="41">
+        <f>E41+F41</f>
+        <v>20</v>
+      </c>
+      <c r="H41" s="22"/>
+    </row>
+    <row r="42" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="26"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D42" s="40">
+        <v>4</v>
+      </c>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="35"/>
+    </row>
+    <row r="43" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="26"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43" s="40">
+        <v>6</v>
+      </c>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="24"/>
+      <c r="H43" s="35"/>
+    </row>
+    <row r="44" spans="1:8" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="25">
+        <v>13</v>
+      </c>
+      <c r="B44" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" s="41"/>
+      <c r="E44" s="27">
+        <v>10</v>
+      </c>
+      <c r="F44" s="27">
+        <v>5</v>
+      </c>
+      <c r="G44" s="41">
+        <f>E44+F44</f>
+        <v>15</v>
+      </c>
+      <c r="H44" s="27"/>
+    </row>
+    <row r="47" spans="1:8" ht="37.200000000000003" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A47" s="48" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C48" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="40">
+        <f>D11+D12+D13+D14</f>
+        <v>402</v>
+      </c>
+      <c r="D49" s="40">
+        <f>C49*150</f>
+        <v>60300</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" s="40">
+        <f>G15+D28+D29+D30+D31+D32</f>
+        <v>163</v>
+      </c>
+      <c r="D50" s="40">
+        <f t="shared" ref="D50:D60" si="0">C50*150</f>
+        <v>24450</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="40">
+        <f>G23+G40+G24</f>
+        <v>133</v>
+      </c>
+      <c r="D51" s="40">
+        <f t="shared" si="0"/>
+        <v>19950</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C52" s="40">
+        <f>G38+G39</f>
+        <v>95</v>
+      </c>
+      <c r="D52" s="40">
+        <f t="shared" si="0"/>
+        <v>14250</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B53" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" s="40">
+        <f>D25+D26+D27</f>
+        <v>17</v>
+      </c>
+      <c r="D53" s="40">
+        <f t="shared" si="0"/>
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C54" s="40">
+        <f>D41+D42</f>
+        <v>14</v>
+      </c>
+      <c r="D54" s="40">
+        <f t="shared" si="0"/>
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B55" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C55" s="40">
+        <f>D41+D43</f>
+        <v>16</v>
+      </c>
+      <c r="D55" s="40">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B56" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C56" s="40">
+        <f>D33+D34+D35</f>
+        <v>25</v>
+      </c>
+      <c r="D56" s="40">
+        <f t="shared" si="0"/>
+        <v>3750</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" s="40">
+        <f>D36+D37+E76+E78</f>
+        <v>77</v>
+      </c>
+      <c r="D57" s="40">
+        <f t="shared" si="0"/>
+        <v>11550</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C58" s="40">
+        <f>D69+D70+D71</f>
+        <v>11</v>
+      </c>
+      <c r="D58" s="40">
+        <f t="shared" si="0"/>
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C59" s="40">
+        <f>D72+D73+D74</f>
+        <v>20.5</v>
+      </c>
+      <c r="D59" s="40">
+        <f t="shared" si="0"/>
+        <v>3075</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B60" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C60" s="40">
+        <f>G44+D75</f>
+        <v>25</v>
+      </c>
+      <c r="D60" s="40">
+        <f t="shared" si="0"/>
+        <v>3750</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B61" s="49"/>
+      <c r="C61" s="50"/>
+      <c r="D61" s="50"/>
+    </row>
+    <row r="62" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B62" s="49"/>
+      <c r="C62" s="50"/>
+      <c r="D62" s="50"/>
+    </row>
+    <row r="64" spans="1:4" ht="37.200000000000003" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="A64" s="48" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D65" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E65" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="F65" s="29"/>
+    </row>
+    <row r="66" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B66" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C66" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="D66" s="41">
+        <v>2</v>
+      </c>
+      <c r="E66" s="41">
+        <f>SUM(D66:D75)</f>
+        <v>50</v>
+      </c>
+      <c r="F66" s="41"/>
+    </row>
+    <row r="67" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="25"/>
+      <c r="B67" s="31"/>
+      <c r="C67" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="D67" s="41">
+        <v>5</v>
+      </c>
+      <c r="E67" s="41"/>
+      <c r="F67" s="41"/>
+    </row>
+    <row r="68" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="25"/>
+      <c r="B68" s="31"/>
+      <c r="C68" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="D68" s="41">
+        <v>1.5</v>
+      </c>
+      <c r="E68" s="41"/>
+      <c r="F68" s="41"/>
+    </row>
+    <row r="69" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="25"/>
+      <c r="B69" s="31"/>
+      <c r="C69" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="D69" s="41">
+        <v>2.5</v>
+      </c>
+      <c r="E69" s="41"/>
+      <c r="F69" s="41"/>
+    </row>
+    <row r="70" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="25"/>
+      <c r="B70" s="31"/>
+      <c r="C70" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="D70" s="41">
+        <v>7</v>
+      </c>
+      <c r="E70" s="41"/>
+      <c r="F70" s="41"/>
+    </row>
+    <row r="71" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="25"/>
+      <c r="B71" s="31"/>
+      <c r="C71" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="D71" s="41">
+        <v>1.5</v>
+      </c>
+      <c r="E71" s="41"/>
+      <c r="F71" s="41"/>
+    </row>
+    <row r="72" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="25"/>
+      <c r="B72" s="31"/>
+      <c r="C72" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="D72" s="41">
+        <v>1</v>
+      </c>
+      <c r="E72" s="41"/>
+      <c r="F72" s="41"/>
+    </row>
+    <row r="73" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="25"/>
+      <c r="B73" s="31"/>
+      <c r="C73" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="D73" s="41">
+        <v>15</v>
+      </c>
+      <c r="E73" s="41"/>
+      <c r="F73" s="41"/>
+    </row>
+    <row r="74" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="25"/>
+      <c r="B74" s="31"/>
+      <c r="C74" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="D74" s="41">
+        <v>4.5</v>
+      </c>
+      <c r="E74" s="41"/>
+      <c r="F74" s="41"/>
+    </row>
+    <row r="75" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="25"/>
+      <c r="B75" s="31"/>
+      <c r="C75" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="D75" s="41">
+        <v>10</v>
+      </c>
+      <c r="E75" s="41"/>
+      <c r="F75" s="41"/>
+    </row>
+    <row r="76" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="B76" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C76" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="D76" s="40">
+        <v>8</v>
+      </c>
+      <c r="E76" s="40">
+        <f>SUM(D76:D77)</f>
+        <v>14</v>
+      </c>
+      <c r="F76" s="46"/>
+    </row>
+    <row r="77" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="26"/>
+      <c r="B77" s="35"/>
+      <c r="C77" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="D77" s="40">
+        <v>6</v>
+      </c>
+      <c r="E77" s="40"/>
+      <c r="F77" s="46"/>
+    </row>
+    <row r="78" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="B78" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="C78" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="D78" s="41">
+        <v>8</v>
+      </c>
+      <c r="E78" s="41">
+        <f>SUM(D78:D79)</f>
+        <v>18</v>
+      </c>
+      <c r="F78" s="27"/>
+    </row>
+    <row r="79" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="31"/>
+      <c r="B79" s="31"/>
+      <c r="C79" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="D79" s="41">
+        <v>10</v>
+      </c>
+      <c r="E79" s="41"/>
+      <c r="F79" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F1EEE5-F282-4D68-B9DB-DC917E7B42A1}">
+  <dimension ref="A2:K32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="26.21875" customWidth="1"/>
+    <col min="4" max="4" width="25.44140625" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:11" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="51" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="J3" s="75" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="78" x14ac:dyDescent="0.3">
+      <c r="A4" s="57" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" s="52" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="59">
+        <v>1</v>
+      </c>
+      <c r="F4" s="59">
+        <v>50</v>
+      </c>
+      <c r="G4" s="62">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>189</v>
+      </c>
+      <c r="K4">
+        <f>$F$23/'takt-time'!B$8</f>
+        <v>0.14153439153439154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="56"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="52" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="63"/>
+      <c r="J5" t="s">
+        <v>190</v>
+      </c>
+      <c r="K5">
+        <f>$F$23/'takt-time'!C$8</f>
+        <v>0.14153439153439154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="58"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="64"/>
+      <c r="J6" t="s">
+        <v>191</v>
+      </c>
+      <c r="K6">
+        <f>$F$23/'takt-time'!D$8</f>
+        <v>0.18871252204585537</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="53"/>
+      <c r="B7" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="E7" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" s="54">
+        <v>1</v>
+      </c>
+      <c r="G7" s="54"/>
+    </row>
+    <row r="8" spans="1:11" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="53"/>
+      <c r="B8" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="F8" s="28">
+        <v>1</v>
+      </c>
+      <c r="G8" s="28"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="65"/>
+      <c r="B9" s="55" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="67" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" s="67" t="s">
+        <v>144</v>
+      </c>
+      <c r="E9" s="67" t="s">
+        <v>137</v>
+      </c>
+      <c r="F9" s="67">
+        <v>1</v>
+      </c>
+      <c r="G9" s="67"/>
+    </row>
+    <row r="10" spans="1:11" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="66"/>
+      <c r="B10" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="68"/>
+    </row>
+    <row r="11" spans="1:11" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="53"/>
+      <c r="B11" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="F11" s="28">
+        <v>1</v>
+      </c>
+      <c r="G11" s="28"/>
+    </row>
+    <row r="12" spans="1:11" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="22"/>
+      <c r="B12" s="54" t="s">
+        <v>148</v>
+      </c>
+      <c r="C12" s="54" t="s">
+        <v>149</v>
+      </c>
+      <c r="D12" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="E12" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="F12" s="54">
+        <v>2</v>
+      </c>
+      <c r="G12" s="54"/>
+    </row>
+    <row r="13" spans="1:11" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="53"/>
+      <c r="B13" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="F13" s="28">
+        <v>2</v>
+      </c>
+      <c r="G13" s="28"/>
+    </row>
+    <row r="14" spans="1:11" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14" s="54" t="s">
+        <v>155</v>
+      </c>
+      <c r="C14" s="54" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="54" t="s">
+        <v>157</v>
+      </c>
+      <c r="E14" s="54">
+        <v>1</v>
+      </c>
+      <c r="F14" s="54">
+        <v>14</v>
+      </c>
+      <c r="G14" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="53"/>
+      <c r="B15" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="F15" s="28">
+        <v>4</v>
+      </c>
+      <c r="G15" s="28"/>
+    </row>
+    <row r="16" spans="1:11" ht="109.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="B16" s="54" t="s">
+        <v>162</v>
+      </c>
+      <c r="C16" s="54" t="s">
+        <v>163</v>
+      </c>
+      <c r="D16" s="54" t="s">
+        <v>164</v>
+      </c>
+      <c r="E16" s="54">
+        <v>1</v>
+      </c>
+      <c r="F16" s="54">
+        <v>18</v>
+      </c>
+      <c r="G16" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="53"/>
+      <c r="B17" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="F17" s="28">
+        <v>1</v>
+      </c>
+      <c r="G17" s="28"/>
+    </row>
+    <row r="18" spans="1:7" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" s="54" t="s">
+        <v>169</v>
+      </c>
+      <c r="C18" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="D18" s="54" t="s">
+        <v>171</v>
+      </c>
+      <c r="E18" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="F18" s="54">
+        <v>3</v>
+      </c>
+      <c r="G18" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="F19" s="28">
+        <v>1</v>
+      </c>
+      <c r="G19" s="28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="22"/>
+      <c r="B20" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="C20" s="54" t="s">
+        <v>177</v>
+      </c>
+      <c r="D20" s="54" t="s">
+        <v>178</v>
+      </c>
+      <c r="E20" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="F20" s="54">
+        <v>4</v>
+      </c>
+      <c r="G20" s="54"/>
+    </row>
+    <row r="21" spans="1:7" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="53"/>
+      <c r="B21" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="F21" s="28">
+        <v>2</v>
+      </c>
+      <c r="G21" s="28"/>
+    </row>
+    <row r="22" spans="1:7" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="B22" s="54" t="s">
+        <v>183</v>
+      </c>
+      <c r="C22" s="54" t="s">
+        <v>184</v>
+      </c>
+      <c r="D22" s="54" t="s">
+        <v>185</v>
+      </c>
+      <c r="E22" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="F22" s="54">
+        <v>2</v>
+      </c>
+      <c r="G22" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="69"/>
+      <c r="F23">
+        <f>SUM(F4:F22)</f>
+        <v>107</v>
+      </c>
+      <c r="G23">
+        <f>SUM(G4:G22)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="69"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="69"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="69"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="69"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="69"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="69"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="69"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="69"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="69"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finishing cost calculation and export to pdf
</commit_message>
<xml_diff>
--- a/3.4 Production Planning/Group 02_WS_25-26 M3 Prodution Planning.xlsx
+++ b/3.4 Production Planning/Group 02_WS_25-26 M3 Prodution Planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\HSRW\Semester 5\Group Project\Group-Project_WS2526\3.4 Production Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B413F4-6068-478D-83EB-0AA22CA95555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD41CA1-4D62-4F32-B730-0DD9EECE7C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="6" xr2:uid="{DE72B6C7-421C-4069-887E-620521B1C591}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{DE72B6C7-421C-4069-887E-620521B1C591}"/>
   </bookViews>
   <sheets>
     <sheet name="takt-time" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="197">
   <si>
     <t>Year 1</t>
   </si>
@@ -737,14 +737,18 @@
   <si>
     <t>Required Assembly Time [h/year]</t>
   </si>
+  <si>
+    <t>Shifts including 3D printing</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.0000"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1031,7 +1035,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1208,6 +1212,18 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1226,17 +1242,8 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="170" fontId="4" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1734,8 +1741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CA06E04-961D-4496-91AB-81E0D50611C9}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E13"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2748,8 +2755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C67BB7A-75CF-4381-AF9B-516380362064}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3019,12 +3026,22 @@
       </c>
       <c r="F14" s="58"/>
     </row>
-    <row r="19" spans="1:6" ht="37.200000000000003" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D15" s="62">
+        <f>SUM(D5:D13)</f>
+        <v>9.1833333333333336</v>
+      </c>
+      <c r="E15" s="62">
+        <f>SUM(E5:E13)</f>
+        <v>1.2244444444444447</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="37.200000000000003" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A19" s="48" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="50" t="s">
         <v>120</v>
       </c>
@@ -3041,7 +3058,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="57" t="s">
         <v>125</v>
       </c>
@@ -3053,7 +3070,7 @@
         <f>B21/252</f>
         <v>0.57539682539682535</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="76">
         <f>C21/7.5</f>
         <v>7.6719576719576715E-2</v>
       </c>
@@ -3062,7 +3079,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="22" t="s">
         <v>151</v>
       </c>
@@ -3074,7 +3091,7 @@
         <f t="shared" ref="C22:C26" si="2">B22/252</f>
         <v>0.17857142857142858</v>
       </c>
-      <c r="D22" s="21">
+      <c r="D22" s="76">
         <f t="shared" ref="D22:D26" si="3">C22/7.5</f>
         <v>2.3809523809523812E-2</v>
       </c>
@@ -3083,7 +3100,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="22" t="s">
         <v>158</v>
       </c>
@@ -3095,7 +3112,7 @@
         <f t="shared" si="2"/>
         <v>0.18849206349206349</v>
       </c>
-      <c r="D23" s="21">
+      <c r="D23" s="76">
         <f t="shared" si="3"/>
         <v>2.5132275132275131E-2</v>
       </c>
@@ -3104,7 +3121,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="22" t="s">
         <v>165</v>
       </c>
@@ -3116,7 +3133,7 @@
         <f t="shared" si="2"/>
         <v>2.976190476190476E-2</v>
       </c>
-      <c r="D24" s="21">
+      <c r="D24" s="76">
         <f t="shared" si="3"/>
         <v>3.968253968253968E-3</v>
       </c>
@@ -3125,7 +3142,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="17" t="s">
         <v>169</v>
       </c>
@@ -3137,7 +3154,7 @@
         <f t="shared" si="2"/>
         <v>6.9444444444444448E-2</v>
       </c>
-      <c r="D25" s="21">
+      <c r="D25" s="76">
         <f t="shared" si="3"/>
         <v>9.2592592592592605E-3</v>
       </c>
@@ -3146,7 +3163,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="22" t="s">
         <v>179</v>
       </c>
@@ -3158,7 +3175,7 @@
         <f t="shared" si="2"/>
         <v>1.984126984126984E-2</v>
       </c>
-      <c r="D26" s="21">
+      <c r="D26" s="76">
         <f t="shared" si="3"/>
         <v>2.6455026455026454E-3</v>
       </c>
@@ -3167,7 +3184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="56"/>
       <c r="C27" s="64">
         <f>SUM(C21:C26)</f>
@@ -3178,36 +3195,50 @@
         <v>0.14153439153439151</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="36.6" x14ac:dyDescent="0.7">
+    <row r="29" spans="1:7" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A29" s="48" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>190</v>
       </c>
       <c r="B30" s="61">
-        <f>_xlfn.CEILING.MATH(C27+D14)</f>
-        <v>17</v>
+        <f>C27+D15</f>
+        <v>10.24484126984127</v>
       </c>
       <c r="C30">
+        <f>_xlfn.CEILING.MATH(B30)</f>
+        <v>11</v>
+      </c>
+      <c r="D30">
         <f>252*B30</f>
-        <v>4284</v>
-      </c>
-      <c r="D30" s="65"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <v>2581.7000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>191</v>
       </c>
-      <c r="B31" s="61">
-        <f>_xlfn.CEILING.MATH(D27+E14)</f>
-        <v>3</v>
-      </c>
-      <c r="C31">
-        <f>252*B31*7.5</f>
-        <v>5670</v>
+      <c r="B31" s="65">
+        <f>D27+E15</f>
+        <v>1.3659788359788361</v>
+      </c>
+      <c r="C31" s="61">
+        <f>_xlfn.CEILING.MATH(B31)</f>
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <f>252*C31*7.5</f>
+        <v>3780</v>
+      </c>
+      <c r="F31" t="s">
+        <v>196</v>
+      </c>
+      <c r="G31" s="61">
+        <f>D27+E14</f>
+        <v>2.2593121693121692</v>
       </c>
     </row>
   </sheetData>
@@ -4497,7 +4528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F1EEE5-F282-4D68-B9DB-DC917E7B42A1}">
   <dimension ref="A2:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -4535,22 +4566,22 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="70" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="73" t="s">
         <v>126</v>
       </c>
-      <c r="C4" s="69" t="s">
+      <c r="C4" s="73" t="s">
         <v>127</v>
       </c>
       <c r="D4" s="51" t="s">
         <v>128</v>
       </c>
-      <c r="E4" s="69">
+      <c r="E4" s="73">
         <v>1</v>
       </c>
-      <c r="F4" s="69">
+      <c r="F4" s="73">
         <v>50</v>
       </c>
       <c r="I4" t="s">
@@ -4562,14 +4593,14 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="67"/>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
+      <c r="A5" s="71"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
       <c r="D5" s="51" t="s">
         <v>129</v>
       </c>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
       <c r="I5" t="s">
         <v>186</v>
       </c>
@@ -4579,14 +4610,14 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="68"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
+      <c r="A6" s="72"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
       <c r="D6" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
       <c r="I6" t="s">
         <v>187</v>
       </c>
@@ -4632,32 +4663,32 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="72"/>
+      <c r="A9" s="66"/>
       <c r="B9" s="54" t="s">
         <v>138</v>
       </c>
-      <c r="C9" s="74" t="s">
+      <c r="C9" s="68" t="s">
         <v>140</v>
       </c>
-      <c r="D9" s="74" t="s">
+      <c r="D9" s="68" t="s">
         <v>141</v>
       </c>
-      <c r="E9" s="74" t="s">
+      <c r="E9" s="68" t="s">
         <v>134</v>
       </c>
-      <c r="F9" s="74">
+      <c r="F9" s="68">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="73"/>
+      <c r="A10" s="67"/>
       <c r="B10" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
     </row>
     <row r="11" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="52"/>
@@ -4921,16 +4952,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>